<commit_message>
notebook working with fitting
</commit_message>
<xml_diff>
--- a/Notebooks/out_gomp_log.xlsx
+++ b/Notebooks/out_gomp_log.xlsx
@@ -781,7 +781,9 @@
           <t>{"A": 11.200201075209062, "mu_m": 0.03581313300057556, "lambda": 104.99780922492452}</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr"/>
+      <c r="Y2" t="n">
+        <v>220.0484447694182</v>
+      </c>
       <c r="Z2" t="inlineStr">
         <is>
           <t>{"A": 11.196747754018519, "mu_m": 0.02683018601181417, "lambda": 41.2167795798658}</t>
@@ -1004,7 +1006,9 @@
           <t>{"A": 11.573075873554416, "mu_m": 0.037935249336114966, "lambda": 96.37783563957743}</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr"/>
+      <c r="Y3" t="n">
+        <v>208.6084591231746</v>
+      </c>
       <c r="Z3" t="inlineStr">
         <is>
           <t>{"A": 11.570237397928551, "mu_m": 0.02812392400097598, "lambda": 30.052793983474093}</t>
@@ -1223,7 +1227,9 @@
           <t>{"A": 11.208070342482154, "mu_m": 0.03717323310883913, "lambda": 102.96838148855674}</t>
         </is>
       </c>
-      <c r="Y4" t="inlineStr"/>
+      <c r="Y4" t="n">
+        <v>213.8874033054168</v>
+      </c>
       <c r="Z4" t="inlineStr">
         <is>
           <t>{"A": 11.205139395276367, "mu_m": 0.027646292518052378, "lambda": 38.636340756046}</t>
@@ -1446,7 +1452,9 @@
           <t>{"A": 11.49980374818283, "mu_m": 0.03792511527681417, "lambda": 85.47207359818246}</t>
         </is>
       </c>
-      <c r="Y5" t="inlineStr"/>
+      <c r="Y5" t="n">
+        <v>197.0219356245514</v>
+      </c>
       <c r="Z5" t="inlineStr">
         <is>
           <t>{"A": 11.497463767590704, "mu_m": 0.027903522549890723, "lambda": 16.483584951126357}</t>
@@ -1665,7 +1673,9 @@
           <t>{"A": 11.168940539654171, "mu_m": 0.03509478333002103, "lambda": 53.479869965974714}</t>
         </is>
       </c>
-      <c r="Y6" t="inlineStr"/>
+      <c r="Y6" t="n">
+        <v>170.5577719882461</v>
+      </c>
       <c r="Z6" t="inlineStr">
         <is>
           <t>{"A": 11.167187389376874, "mu_m": 0.02551605172437022, "lambda": -24.162918158457664}</t>
@@ -1884,7 +1894,9 @@
           <t>{"A": 11.448802863792606, "mu_m": 0.038599929763779774, "lambda": 106.51338392374262}</t>
         </is>
       </c>
-      <c r="Y7" t="inlineStr"/>
+      <c r="Y7" t="n">
+        <v>215.6270332331814</v>
+      </c>
       <c r="Z7" t="inlineStr">
         <is>
           <t>{"A": 11.445627916682135, "mu_m": 0.028897608136177977, "lambda": 45.695217811707664}</t>
@@ -2103,7 +2115,9 @@
           <t>{"A": 11.206545042794875, "mu_m": 0.037636849558578454, "lambda": 106.49990471116979}</t>
         </is>
       </c>
-      <c r="Y8" t="inlineStr"/>
+      <c r="Y8" t="n">
+        <v>216.0377001472469</v>
+      </c>
       <c r="Z8" t="inlineStr">
         <is>
           <t>{"A": 11.203632472199786, "mu_m": 0.027998069321336933, "lambda": 43.07119431468285}</t>
@@ -2322,7 +2336,9 @@
           <t>{"A": 10.53018154874278, "mu_m": 0.028027222026921556, "lambda": 86.50701260506892}</t>
         </is>
       </c>
-      <c r="Y9" t="inlineStr"/>
+      <c r="Y9" t="n">
+        <v>224.7239682442797</v>
+      </c>
       <c r="Z9" t="inlineStr">
         <is>
           <t>{"A": 10.52465358219776, "mu_m": 0.021352154571379185, "lambda": 17.439912694053074}</t>
@@ -2533,7 +2549,9 @@
           <t>{"A": 10.028886316969949, "mu_m": 0.025842272894417064, "lambda": 113.26936039323274}</t>
         </is>
       </c>
-      <c r="Y10" t="inlineStr"/>
+      <c r="Y10" t="n">
+        <v>256.0362566694457</v>
+      </c>
       <c r="Z10" t="inlineStr">
         <is>
           <t>{"A": 10.021145606707497, "mu_m": 0.020074872865894416, "lambda": 50.57373825018106}</t>
@@ -2756,7 +2774,9 @@
           <t>{"A": 12.966038580997843, "mu_m": 0.030646291671127705, "lambda": 47.39222077510513}</t>
         </is>
       </c>
-      <c r="Y11" t="inlineStr"/>
+      <c r="Y11" t="n">
+        <v>203.0371215863401</v>
+      </c>
       <c r="Z11" t="inlineStr">
         <is>
           <t>{"A": 12.955022917154091, "mu_m": 0.023691499227940456, "lambda": -23.491133211425435}</t>
@@ -2977,7 +2997,9 @@
           <t>{"A": 12.760130824396162, "mu_m": 0.03776327342967258, "lambda": 156.1305368351974}</t>
         </is>
       </c>
-      <c r="Y12" t="inlineStr"/>
+      <c r="Y12" t="n">
+        <v>280.4362278049025</v>
+      </c>
       <c r="Z12" t="inlineStr">
         <is>
           <t>{"A": 12.748297934573438, "mu_m": 0.030142875638081497, "lambda": 112.49276452173477}</t>
@@ -3200,7 +3222,9 @@
           <t>{"A": 12.400784732820625, "mu_m": 0.029827585942767246, "lambda": 69.45534396388402}</t>
         </is>
       </c>
-      <c r="Y13" t="inlineStr"/>
+      <c r="Y13" t="n">
+        <v>222.4008007752698</v>
+      </c>
       <c r="Z13" t="inlineStr">
         <is>
           <t>{"A": 12.388652345347431, "mu_m": 0.02341098614514121, "lambda": 6.804302950757791}</t>
@@ -3423,7 +3447,9 @@
           <t>{"A": 12.245483394053743, "mu_m": 0.027430503301719096, "lambda": 0.8504503467337587}</t>
         </is>
       </c>
-      <c r="Y14" t="inlineStr"/>
+      <c r="Y14" t="n">
+        <v>165.078628675359</v>
+      </c>
       <c r="Z14" t="inlineStr">
         <is>
           <t>{"A": 12.241304287944054, "mu_m": 0.020186720989920335, "lambda": -100.76243660079186}</t>
@@ -3646,7 +3672,9 @@
           <t>{"A": 12.523453956176308, "mu_m": 0.030378759935668215, "lambda": 13.819193833817302}</t>
         </is>
       </c>
-      <c r="Y15" t="inlineStr"/>
+      <c r="Y15" t="n">
+        <v>165.4751946939818</v>
+      </c>
       <c r="Z15" t="inlineStr">
         <is>
           <t>{"A": 12.520074440166942, "mu_m": 0.022231830179475682, "lambda": -83.13927816124237}</t>
@@ -3869,7 +3897,9 @@
           <t>{"A": 12.649956501494174, "mu_m": 0.03048638696354454, "lambda": 7.071680456063442}</t>
         </is>
       </c>
-      <c r="Y16" t="inlineStr"/>
+      <c r="Y16" t="n">
+        <v>159.7187925647417</v>
+      </c>
       <c r="Z16" t="inlineStr">
         <is>
           <t>{"A": 12.646701595733175, "mu_m": 0.022260698750394686, "lambda": -91.80701056145153}</t>
@@ -4092,7 +4122,9 @@
           <t>{"A": 12.444527935224556, "mu_m": 0.0275734282044631, "lambda": 3.036522984628338}</t>
         </is>
       </c>
-      <c r="Y17" t="inlineStr"/>
+      <c r="Y17" t="n">
+        <v>169.0690506959194</v>
+      </c>
       <c r="Z17" t="inlineStr">
         <is>
           <t>{"A": 12.43990962074963, "mu_m": 0.020344115920339516, "lambda": -98.16897849780113}</t>
@@ -4315,7 +4347,9 @@
           <t>{"A": 12.470570340482704, "mu_m": 0.030281669426873364, "lambda": 7.8252882371520185}</t>
         </is>
       </c>
-      <c r="Y18" t="inlineStr"/>
+      <c r="Y18" t="n">
+        <v>159.3250745690981</v>
+      </c>
       <c r="Z18" t="inlineStr">
         <is>
           <t>{"A": 12.4673552538348, "mu_m": 0.022119670345906436, "lambda": -90.12882300154233}</t>
@@ -4538,7 +4572,9 @@
           <t>{"A": 12.549020682099751, "mu_m": 0.029740062751884167, "lambda": -1.9259896952747126}</t>
         </is>
       </c>
-      <c r="Y19" t="inlineStr"/>
+      <c r="Y19" t="n">
+        <v>153.3032293650398</v>
+      </c>
       <c r="Z19" t="inlineStr">
         <is>
           <t>{"A": 12.545760665770443, "mu_m": 0.02169898234731017, "lambda": -102.97851360143969}</t>
@@ -4761,7 +4797,9 @@
           <t>{"A": 13.09196387647755, "mu_m": 0.01596579922475536, "lambda": -283.9084442062667}</t>
         </is>
       </c>
-      <c r="Y20" t="inlineStr"/>
+      <c r="Y20" t="n">
+        <v>17.75289368952343</v>
+      </c>
       <c r="Z20" t="inlineStr">
         <is>
           <t>{"A": 13.082838555685267, "mu_m": 0.011669714955758028, "lambda": -479.05360660531466}</t>
@@ -4984,7 +5022,9 @@
           <t>{"A": 12.777067090013578, "mu_m": 0.029602673017193985, "lambda": 20.42453548917942}</t>
         </is>
       </c>
-      <c r="Y21" t="inlineStr"/>
+      <c r="Y21" t="n">
+        <v>179.2081797281337</v>
+      </c>
       <c r="Z21" t="inlineStr">
         <is>
           <t>{"A": 12.773648099433514, "mu_m": 0.021620596809268002, "lambda": -82.21970611516927}</t>
@@ -5207,7 +5247,9 @@
           <t>{"A": 13.260277118286098, "mu_m": 0.023841402005867554, "lambda": -9.268804680747493}</t>
         </is>
       </c>
-      <c r="Y22" t="inlineStr"/>
+      <c r="Y22" t="n">
+        <v>195.3409466607632</v>
+      </c>
       <c r="Z22" t="inlineStr">
         <is>
           <t>{"A": 13.252131581325056, "mu_m": 0.017750446130706747, "lambda": -127.57698358803687}</t>
@@ -5430,7 +5472,9 @@
           <t>{"A": 13.58239764701819, "mu_m": 0.020996102008565977, "lambda": -53.99109251188165}</t>
         </is>
       </c>
-      <c r="Y23" t="inlineStr"/>
+      <c r="Y23" t="n">
+        <v>183.9904554018607</v>
+      </c>
       <c r="Z23" t="inlineStr">
         <is>
           <t>{"A": 13.569503252546802, "mu_m": 0.015767470067281478, "lambda": -185.13690426041882}</t>
@@ -5653,7 +5697,9 @@
           <t>{"A": 13.49423288192887, "mu_m": 0.021153060930772002, "lambda": -30.7315929231626}</t>
         </is>
       </c>
-      <c r="Y24" t="inlineStr"/>
+      <c r="Y24" t="n">
+        <v>203.9507950247512</v>
+      </c>
       <c r="Z24" t="inlineStr">
         <is>
           <t>{"A": 13.479864113324052, "mu_m": 0.01600013772427815, "lambda": -154.50397395453123}</t>
@@ -5876,7 +5922,9 @@
           <t>{"A": 11.902934467615001, "mu_m": 0.032318237831638716, "lambda": 164.61677628244325}</t>
         </is>
       </c>
-      <c r="Y25" t="inlineStr"/>
+      <c r="Y25" t="n">
+        <v>300.1082255086671</v>
+      </c>
       <c r="Z25" t="inlineStr">
         <is>
           <t>{"A": 11.893970052301814, "mu_m": 0.02521192144555857, "lambda": 107.05048594609035}</t>
@@ -6099,7 +6147,9 @@
           <t>{"A": 11.90894643224164, "mu_m": 0.03325704745846213, "lambda": 177.27111369399736}</t>
         </is>
       </c>
-      <c r="Y26" t="inlineStr"/>
+      <c r="Y26" t="n">
+        <v>309.0042918694086</v>
+      </c>
       <c r="Z26" t="inlineStr">
         <is>
           <t>{"A": 11.899417962659879, "mu_m": 0.026146419748896987, "lambda": 124.29891925351768}</t>
@@ -6322,7 +6372,9 @@
           <t>{"A": 11.95643759277621, "mu_m": 0.026570213621625895, "lambda": 92.21693593137569}</t>
         </is>
       </c>
-      <c r="Y27" t="inlineStr"/>
+      <c r="Y27" t="n">
+        <v>257.7604894258689</v>
+      </c>
       <c r="Z27" t="inlineStr">
         <is>
           <t>{"A": 11.946917747574656, "mu_m": 0.020362063912955138, "lambda": 12.415212189186512}</t>
@@ -6545,7 +6597,9 @@
           <t>{"A": 11.960419488853304, "mu_m": 0.025536184079924723, "lambda": 75.20980757705979}</t>
         </is>
       </c>
-      <c r="Y28" t="inlineStr"/>
+      <c r="Y28" t="n">
+        <v>247.5140337670032</v>
+      </c>
       <c r="Z28" t="inlineStr">
         <is>
           <t>{"A": 11.951211953379893, "mu_m": 0.01950228910354624, "lambda": -9.6496102262956}</t>
@@ -6768,7 +6822,9 @@
           <t>{"A": 11.938831605042779, "mu_m": 0.04820612332084526, "lambda": 301.47967538090603}</t>
         </is>
       </c>
-      <c r="Y29" t="inlineStr"/>
+      <c r="Y29" t="n">
+        <v>392.589484603086</v>
+      </c>
       <c r="Z29" t="inlineStr">
         <is>
           <t>{"A": 11.911890015688364, "mu_m": 0.04274800174115042, "lambda": 289.5231042349278}</t>
@@ -6991,7 +7047,9 @@
           <t>{"A": 12.41294547245797, "mu_m": 0.029879563032072898, "lambda": 93.45762529850653}</t>
         </is>
       </c>
-      <c r="Y30" t="inlineStr"/>
+      <c r="Y30" t="n">
+        <v>246.2867492986718</v>
+      </c>
       <c r="Z30" t="inlineStr">
         <is>
           <t>{"A": 12.405653534302694, "mu_m": 0.022644912216965667, "lambda": 14.42526959338689}</t>
@@ -7214,7 +7272,9 @@
           <t>{"A": 12.794912187637951, "mu_m": 0.028478750218534524, "lambda": 66.26828069618611}</t>
         </is>
       </c>
-      <c r="Y31" t="inlineStr"/>
+      <c r="Y31" t="n">
+        <v>231.5488884934528</v>
+      </c>
       <c r="Z31" t="inlineStr">
         <is>
           <t>{"A": 12.787245973741785, "mu_m": 0.021531612149823923, "lambda": -20.47036702370947}</t>
@@ -7437,7 +7497,9 @@
           <t>{"A": 11.920426169842846, "mu_m": 0.027453671816229173, "lambda": 100.89422274013374}</t>
         </is>
       </c>
-      <c r="Y32" t="inlineStr"/>
+      <c r="Y32" t="n">
+        <v>260.6280371181025</v>
+      </c>
       <c r="Z32" t="inlineStr">
         <is>
           <t>{"A": 11.911880403245815, "mu_m": 0.0210085713583274, "lambda": 23.362893557916955}</t>
@@ -7660,7 +7722,9 @@
           <t>{"A": 11.968416821872111, "mu_m": 0.024573615050696666, "lambda": 57.171056768462364}</t>
         </is>
       </c>
-      <c r="Y33" t="inlineStr"/>
+      <c r="Y33" t="n">
+        <v>236.344307552025</v>
+      </c>
       <c r="Z33" t="inlineStr">
         <is>
           <t>{"A": 11.958812676558995, "mu_m": 0.018737727601983972, "lambda": -32.16208054955169}</t>
@@ -7883,7 +7947,9 @@
           <t>{"A": 12.594388638582016, "mu_m": 0.030236800647414387, "lambda": 99.4679543074649}</t>
         </is>
       </c>
-      <c r="Y34" t="inlineStr"/>
+      <c r="Y34" t="n">
+        <v>252.6990024029488</v>
+      </c>
       <c r="Z34" t="inlineStr">
         <is>
           <t>{"A": 12.58610357359597, "mu_m": 0.02308348039743714, "lambda": 23.749002733374024}</t>
@@ -8106,7 +8172,9 @@
           <t>{"A": 11.837665703916311, "mu_m": 0.024629895098126218, "lambda": 78.16096841886588}</t>
         </is>
       </c>
-      <c r="Y35" t="inlineStr"/>
+      <c r="Y35" t="n">
+        <v>254.971865362653</v>
+      </c>
       <c r="Z35" t="inlineStr">
         <is>
           <t>{"A": 11.826971986429559, "mu_m": 0.018963775134492142, "lambda": -4.53206792504828}</t>
@@ -8368,7 +8436,9 @@
           <t>{"A": 13.424843268013953, "mu_m": 0.027261735707643283, "lambda": 26.403658406330674}</t>
         </is>
       </c>
-      <c r="Y36" t="inlineStr"/>
+      <c r="Y36" t="n">
+        <v>207.563210835948</v>
+      </c>
       <c r="Z36" t="inlineStr">
         <is>
           <t>{"A": 13.420703721696828, "mu_m": 0.020187426815930564, "lambda": -81.38467473329949}</t>
@@ -8630,7 +8700,9 @@
           <t>{"A": 13.083861369165763, "mu_m": 0.025034960325727707, "lambda": 3.8454304756805}</t>
         </is>
       </c>
-      <c r="Y37" t="inlineStr"/>
+      <c r="Y37" t="n">
+        <v>196.1079124699839</v>
+      </c>
       <c r="Z37" t="inlineStr">
         <is>
           <t>{"A": 13.07953282703733, "mu_m": 0.018534121817810282, "lambda": -110.75645089703237}</t>
@@ -8892,7 +8964,9 @@
           <t>{"A": 13.224119386925734, "mu_m": 0.03225191857751883, "lambda": 107.30103360325796}</t>
         </is>
       </c>
-      <c r="Y38" t="inlineStr"/>
+      <c r="Y38" t="n">
+        <v>258.141103422786</v>
+      </c>
       <c r="Z38" t="inlineStr">
         <is>
           <t>{"A": 13.219796942255492, "mu_m": 0.02421370137136143, "lambda": 24.79283116929131}</t>
@@ -9154,7 +9228,9 @@
           <t>{"A": 13.21880845806345, "mu_m": 0.02504366238047861, "lambda": 27.79973303223087}</t>
         </is>
       </c>
-      <c r="Y39" t="inlineStr"/>
+      <c r="Y39" t="n">
+        <v>221.9777168520152</v>
+      </c>
       <c r="Z39" t="inlineStr">
         <is>
           <t>{"A": 13.21302730495696, "mu_m": 0.018762404775559936, "lambda": -79.96338210780564}</t>
@@ -9416,7 +9492,9 @@
           <t>{"A": 12.650402853660513, "mu_m": 0.02466954437006436, "lambda": 13.36754459664763}</t>
         </is>
       </c>
-      <c r="Y40" t="inlineStr"/>
+      <c r="Y40" t="n">
+        <v>202.0140417749864</v>
+      </c>
       <c r="Z40" t="inlineStr">
         <is>
           <t>{"A": 12.64604935625848, "mu_m": 0.01829215357343214, "lambda": -98.12587892659572}</t>
@@ -9678,7 +9756,9 @@
           <t>{"A": 13.072637806362009, "mu_m": 0.027500071236951036, "lambda": 39.97801026362594}</t>
         </is>
       </c>
-      <c r="Y41" t="inlineStr"/>
+      <c r="Y41" t="n">
+        <v>214.8559096480903</v>
+      </c>
       <c r="Z41" t="inlineStr">
         <is>
           <t>{"A": 13.068495718561604, "mu_m": 0.020379436563794966, "lambda": -63.72782672632222}</t>
@@ -9940,7 +10020,9 @@
           <t>{"A": 13.35583713535338, "mu_m": 0.01870311085101847, "lambda": 113.8897253040232}</t>
         </is>
       </c>
-      <c r="Y42" t="inlineStr"/>
+      <c r="Y42" t="n">
+        <v>376.5913657353018</v>
+      </c>
       <c r="Z42" t="inlineStr">
         <is>
           <t>{"A": 13.324591288258132, "mu_m": 0.015412590108580223, "lambda": 40.34079206130854}</t>
@@ -10159,7 +10241,9 @@
           <t>{"A": 11.141237958519277, "mu_m": 0.035593666496416966, "lambda": 113.4020080439888}</t>
         </is>
       </c>
-      <c r="Y43" t="inlineStr"/>
+      <c r="Y43" t="n">
+        <v>228.5526176208561</v>
+      </c>
       <c r="Z43" t="inlineStr">
         <is>
           <t>{"A": 11.140639559301283, "mu_m": 0.025046954473591697, "lambda": 20.998362936629846}</t>
@@ -10378,7 +10462,9 @@
           <t>{"A": 11.27414401474435, "mu_m": 0.036944693986843, "lambda": 118.56471243385568}</t>
         </is>
       </c>
-      <c r="Y44" t="inlineStr"/>
+      <c r="Y44" t="n">
+        <v>230.8278103852844</v>
+      </c>
       <c r="Z44" t="inlineStr">
         <is>
           <t>{"A": 11.273646652835573, "mu_m": 0.025949638256129507, "lambda": 27.58926878885701}</t>
@@ -10597,7 +10683,9 @@
           <t>{"A": 10.781262725245604, "mu_m": 0.02961805116324555, "lambda": 85.96676468797999}</t>
         </is>
       </c>
-      <c r="Y45" t="inlineStr"/>
+      <c r="Y45" t="n">
+        <v>219.8785094082979</v>
+      </c>
       <c r="Z45" t="inlineStr">
         <is>
           <t>{"A": 10.780558309141886, "mu_m": 0.020919643323828185, "lambda": -18.956677501512612}</t>
@@ -10816,7 +10904,9 @@
           <t>{"A": 10.687980057477285, "mu_m": 0.02500682380951449, "lambda": 24.988091743042364}</t>
         </is>
       </c>
-      <c r="Y46" t="inlineStr"/>
+      <c r="Y46" t="n">
+        <v>182.2206999601753</v>
+      </c>
       <c r="Z46" t="inlineStr">
         <is>
           <t>{"A": 10.686942407818924, "mu_m": 0.017703341821430723, "lambda": -96.78306175740995}</t>
@@ -11035,7 +11125,9 @@
           <t>{"A": 10.596477525234196, "mu_m": 0.028031712575196738, "lambda": 85.61777675528892}</t>
         </is>
       </c>
-      <c r="Y47" t="inlineStr"/>
+      <c r="Y47" t="n">
+        <v>224.6826383798393</v>
+      </c>
       <c r="Z47" t="inlineStr">
         <is>
           <t>{"A": 10.595509660347917, "mu_m": 0.01989048119382012, "lambda": -20.59726549612036}</t>
@@ -11254,7 +11346,9 @@
           <t>{"A": 10.638702409629476, "mu_m": 0.029639281582672164, "lambda": 118.32227487491316}</t>
         </is>
       </c>
-      <c r="Y48" t="inlineStr"/>
+      <c r="Y48" t="n">
+        <v>250.3686568470001</v>
+      </c>
       <c r="Z48" t="inlineStr">
         <is>
           <t>{"A": 10.637594179622091, "mu_m": 0.02112504812914626, "lambda": 20.022892295221997}</t>
@@ -11473,7 +11567,9 @@
           <t>{"A": 10.694046286086644, "mu_m": 0.028844171721437908, "lambda": 95.04921685045765}</t>
         </is>
       </c>
-      <c r="Y49" t="inlineStr"/>
+      <c r="Y49" t="n">
+        <v>231.4414076049985</v>
+      </c>
       <c r="Z49" t="inlineStr">
         <is>
           <t>{"A": 10.693088452628206, "mu_m": 0.020474978923621743, "lambda": -8.861061167060441}</t>
@@ -11692,7 +11788,9 @@
           <t>{"A": 10.863374184063737, "mu_m": 0.03773142144363917, "lambda": 190.3937985896372}</t>
         </is>
       </c>
-      <c r="Y50" t="inlineStr"/>
+      <c r="Y50" t="n">
+        <v>296.3111446943747</v>
+      </c>
       <c r="Z50" t="inlineStr">
         <is>
           <t>{"A": 10.862233287321063, "mu_m": 0.027062291339038817, "lambda": 114.24279530206324}</t>
@@ -11911,7 +12009,9 @@
           <t>{"A": 11.127591050945886, "mu_m": 0.03665469465226248, "lambda": 153.6233130182189}</t>
         </is>
       </c>
-      <c r="Y51" t="inlineStr"/>
+      <c r="Y51" t="n">
+        <v>265.3037407571973</v>
+      </c>
       <c r="Z51" t="inlineStr">
         <is>
           <t>{"A": 11.126654119153354, "mu_m": 0.026054322925039907, "lambda": 69.00760268996326}</t>
@@ -12130,7 +12230,9 @@
           <t>{"A": 11.146816863947757, "mu_m": 0.04135384286607107, "lambda": 207.09102633774563}</t>
         </is>
       </c>
-      <c r="Y52" t="inlineStr"/>
+      <c r="Y52" t="n">
+        <v>306.2519379857882</v>
+      </c>
       <c r="Z52" t="inlineStr">
         <is>
           <t>{"A": 11.145952945359896, "mu_m": 0.02956391697138099, "lambda": 134.6337671458744}</t>
@@ -12353,7 +12455,9 @@
           <t>{"A": 12.372171997611135, "mu_m": 0.032623065066345415, "lambda": 124.43347470297749}</t>
         </is>
       </c>
-      <c r="Y53" t="inlineStr"/>
+      <c r="Y53" t="n">
+        <v>263.9503383484334</v>
+      </c>
       <c r="Z53" t="inlineStr">
         <is>
           <t>{"A": 12.368531723395822, "mu_m": 0.02408463886772064, "lambda": 39.754473573511504}</t>
@@ -12576,7 +12680,9 @@
           <t>{"A": 12.588514794522728, "mu_m": 0.0325749235171165, "lambda": 93.12507249166734}</t>
         </is>
       </c>
-      <c r="Y54" t="inlineStr"/>
+      <c r="Y54" t="n">
+        <v>235.2913552568154</v>
+      </c>
       <c r="Z54" t="inlineStr">
         <is>
           <t>{"A": 12.585754510763323, "mu_m": 0.023740248774793922, "lambda": 0.01359364089102528}</t>
@@ -12799,7 +12905,9 @@
           <t>{"A": 12.091704819101933, "mu_m": 0.03260154935656442, "lambda": 138.1375458911161}</t>
         </is>
       </c>
-      <c r="Y55" t="inlineStr"/>
+      <c r="Y55" t="n">
+        <v>274.5816627951975</v>
+      </c>
       <c r="Z55" t="inlineStr">
         <is>
           <t>{"A": 12.087801309820298, "mu_m": 0.024170344364379714, "lambda": 57.33018947387293}</t>
@@ -13022,7 +13130,9 @@
           <t>{"A": 12.816555425714101, "mu_m": 0.03547608254907496, "lambda": 156.06044469074496}</t>
         </is>
       </c>
-      <c r="Y56" t="inlineStr"/>
+      <c r="Y56" t="n">
+        <v>288.9654023120442</v>
+      </c>
       <c r="Z56" t="inlineStr">
         <is>
           <t>{"A": 12.812251876648563, "mu_m": 0.026434809971677107, "lambda": 79.83356767481916}</t>
@@ -13245,7 +13355,9 @@
           <t>{"A": 12.462497978877806, "mu_m": 0.03234369919028809, "lambda": 123.97509910290407}</t>
         </is>
       </c>
-      <c r="Y57" t="inlineStr"/>
+      <c r="Y57" t="n">
+        <v>265.7244013424714</v>
+      </c>
       <c r="Z57" t="inlineStr">
         <is>
           <t>{"A": 12.458632319363518, "mu_m": 0.023916205371534667, "lambda": 38.76516240481342}</t>
@@ -13468,7 +13580,9 @@
           <t>{"A": 12.263822450296813, "mu_m": 0.03128124817574032, "lambda": 102.01038747602334}</t>
         </is>
       </c>
-      <c r="Y58" t="inlineStr"/>
+      <c r="Y58" t="n">
+        <v>246.2376294420228</v>
+      </c>
       <c r="Z58" t="inlineStr">
         <is>
           <t>{"A": 12.26060090374553, "mu_m": 0.022930480398947677, "lambda": 10.696479136243502}</t>
@@ -13691,7 +13805,9 @@
           <t>{"A": 12.321832806074726, "mu_m": 0.02965506110041603, "lambda": 115.03850558644368}</t>
         </is>
       </c>
-      <c r="Y59" t="inlineStr"/>
+      <c r="Y59" t="n">
+        <v>267.8943352054602</v>
+      </c>
       <c r="Z59" t="inlineStr">
         <is>
           <t>{"A": 12.317303629667178, "mu_m": 0.022003200427819815, "lambda": 25.097866050732417}</t>
@@ -13914,7 +14030,9 @@
           <t>{"A": 12.112728282850824, "mu_m": 0.02810091168829989, "lambda": 76.58677390638572}</t>
         </is>
       </c>
-      <c r="Y60" t="inlineStr"/>
+      <c r="Y60" t="n">
+        <v>235.1589854126764</v>
+      </c>
       <c r="Z60" t="inlineStr">
         <is>
           <t>{"A": 12.10911786281607, "mu_m": 0.020606679958755005, "lambda": -23.563350260665725}</t>
@@ -14137,7 +14255,9 @@
           <t>{"A": 12.299511438226522, "mu_m": 0.027440138788513986, "lambda": 74.81399866551634}</t>
         </is>
       </c>
-      <c r="Y61" t="inlineStr"/>
+      <c r="Y61" t="n">
+        <v>239.7088422903788</v>
+      </c>
       <c r="Z61" t="inlineStr">
         <is>
           <t>{"A": 12.295304380848012, "mu_m": 0.0202193608220603, "lambda": -26.350808790360272}</t>
@@ -14360,7 +14480,9 @@
           <t>{"A": 12.472295461551202, "mu_m": 0.029613962711674553, "lambda": 104.11907519669892}</t>
         </is>
       </c>
-      <c r="Y62" t="inlineStr"/>
+      <c r="Y62" t="n">
+        <v>259.0561610974572</v>
+      </c>
       <c r="Z62" t="inlineStr">
         <is>
           <t>{"A": 12.46770914150766, "mu_m": 0.02195966272148072, "lambda": 12.53018573472463}</t>
@@ -14583,7 +14705,9 @@
           <t>{"A": 12.319784353466877, "mu_m": 0.02890703056069677, "lambda": 103.07361248720278}</t>
         </is>
       </c>
-      <c r="Y63" t="inlineStr"/>
+      <c r="Y63" t="n">
+        <v>259.8588406962959</v>
+      </c>
       <c r="Z63" t="inlineStr">
         <is>
           <t>{"A": 12.315187514738543, "mu_m": 0.021444445910861372, "lambda": 10.672539862510346}</t>
@@ -14806,7 +14930,9 @@
           <t>{"A": 12.690189125027977, "mu_m": 0.023138099778236262, "lambda": 41.313481298928494}</t>
         </is>
       </c>
-      <c r="Y64" t="inlineStr"/>
+      <c r="Y64" t="n">
+        <v>243.0785237362668</v>
+      </c>
       <c r="Z64" t="inlineStr">
         <is>
           <t>{"A": 12.681370006548454, "mu_m": 0.01735415310177329, "lambda": -70.35698451955997}</t>
@@ -15029,7 +15155,9 @@
           <t>{"A": 12.349674952922262, "mu_m": 0.023382603992888062, "lambda": 34.45093664094444}</t>
         </is>
       </c>
-      <c r="Y65" t="inlineStr"/>
+      <c r="Y65" t="n">
+        <v>228.7488652083459</v>
+      </c>
       <c r="Z65" t="inlineStr">
         <is>
           <t>{"A": 12.342722718553611, "mu_m": 0.01737614007790205, "lambda": -79.309350715746}</t>
@@ -15252,7 +15380,9 @@
           <t>{"A": 12.517370173358657, "mu_m": 0.02358935356859548, "lambda": 59.534445908138636}</t>
         </is>
       </c>
-      <c r="Y66" t="inlineStr"/>
+      <c r="Y66" t="n">
+        <v>254.744676274169</v>
+      </c>
       <c r="Z66" t="inlineStr">
         <is>
           <t>{"A": 12.508546141142286, "mu_m": 0.017746609994047268, "lambda": -46.498649151351486}</t>
@@ -15475,7 +15605,9 @@
           <t>{"A": 11.58363603611944, "mu_m": 0.03394116321648483, "lambda": 106.04120431323516}</t>
         </is>
       </c>
-      <c r="Y67" t="inlineStr"/>
+      <c r="Y67" t="n">
+        <v>231.5932228024334</v>
+      </c>
       <c r="Z67" t="inlineStr">
         <is>
           <t>{"A": 11.579155559453786, "mu_m": 0.025557234967466872, "lambda": 38.57280917063295}</t>
@@ -15698,7 +15830,9 @@
           <t>{"A": 11.567753683006869, "mu_m": 0.033111730539068615, "lambda": 106.54209527133304}</t>
         </is>
       </c>
-      <c r="Y68" t="inlineStr"/>
+      <c r="Y68" t="n">
+        <v>235.0626736655169</v>
+      </c>
       <c r="Z68" t="inlineStr">
         <is>
           <t>{"A": 11.562780873183202, "mu_m": 0.025066122957507472, "lambda": 39.75254227527662}</t>
@@ -15921,7 +16055,9 @@
           <t>{"A": 11.826793008263015, "mu_m": 0.035097028233578825, "lambda": 151.62022387634565}</t>
         </is>
       </c>
-      <c r="Y69" t="inlineStr"/>
+      <c r="Y69" t="n">
+        <v>275.5861042287879</v>
+      </c>
       <c r="Z69" t="inlineStr">
         <is>
           <t>{"A": 11.819328334135369, "mu_m": 0.02723323149234042, "lambda": 96.92512680317856}</t>
@@ -16144,7 +16280,9 @@
           <t>{"A": 11.783379064708006, "mu_m": 0.03348878248676743, "lambda": 122.92954281524607}</t>
         </is>
       </c>
-      <c r="Y70" t="inlineStr"/>
+      <c r="Y70" t="n">
+        <v>252.3717793954773</v>
+      </c>
       <c r="Z70" t="inlineStr">
         <is>
           <t>{"A": 11.776820964172995, "mu_m": 0.025694838188239928, "lambda": 61.17202787458726}</t>
@@ -16367,7 +16505,9 @@
           <t>{"A": 12.052638225671506, "mu_m": 0.03475536333941755, "lambda": 116.70606424963158}</t>
         </is>
       </c>
-      <c r="Y71" t="inlineStr"/>
+      <c r="Y71" t="n">
+        <v>244.2811314932216</v>
+      </c>
       <c r="Z71" t="inlineStr">
         <is>
           <t>{"A": 12.046853766149988, "mu_m": 0.026444954360924554, "lambda": 52.487282808398994}</t>
@@ -16590,7 +16730,9 @@
           <t>{"A": 12.166246449855688, "mu_m": 0.03570353562836665, "lambda": 126.27862874228734}</t>
         </is>
       </c>
-      <c r="Y72" t="inlineStr"/>
+      <c r="Y72" t="n">
+        <v>251.6362961653136</v>
+      </c>
       <c r="Z72" t="inlineStr">
         <is>
           <t>{"A": 12.160334025725955, "mu_m": 0.02724121256363794, "lambda": 64.3729886375597}</t>
@@ -16809,7 +16951,9 @@
           <t>{"A": 11.432730249753968, "mu_m": 0.03212223614302613, "lambda": 106.4166066401869}</t>
         </is>
       </c>
-      <c r="Y73" t="inlineStr"/>
+      <c r="Y73" t="n">
+        <v>237.3497831667671</v>
+      </c>
       <c r="Z73" t="inlineStr">
         <is>
           <t>{"A": 11.427312241799543, "mu_m": 0.02439218785177117, "lambda": 39.626579033259326}</t>
@@ -17028,7 +17172,9 @@
           <t>{"A": 11.275751706735942, "mu_m": 0.03162848843712144, "lambda": 91.20046092592641}</t>
         </is>
       </c>
-      <c r="Y74" t="inlineStr"/>
+      <c r="Y74" t="n">
+        <v>222.3517565342689</v>
+      </c>
       <c r="Z74" t="inlineStr">
         <is>
           <t>{"A": 11.270977822766914, "mu_m": 0.02381963182301306, "lambda": 20.594747741525396}</t>
@@ -17247,7 +17393,9 @@
           <t>{"A": 11.316205074516565, "mu_m": 0.03142300292391474, "lambda": 92.18784283519601}</t>
         </is>
       </c>
-      <c r="Y75" t="inlineStr"/>
+      <c r="Y75" t="n">
+        <v>224.6703814733575</v>
+      </c>
       <c r="Z75" t="inlineStr">
         <is>
           <t>{"A": 11.311568619705636, "mu_m": 0.02363014169757959, "lambda": 20.363170011168794}</t>
@@ -17470,7 +17618,9 @@
           <t>{"A": 11.509885677701629, "mu_m": 0.03245793772580804, "lambda": 99.59255082241712}</t>
         </is>
       </c>
-      <c r="Y76" t="inlineStr"/>
+      <c r="Y76" t="n">
+        <v>230.04601175482</v>
+      </c>
       <c r="Z76" t="inlineStr">
         <is>
           <t>{"A": 11.50496119160834, "mu_m": 0.02447313031758038, "lambda": 29.996208545461155}</t>
@@ -17693,7 +17843,9 @@
           <t>{"A": 11.51086986502326, "mu_m": 0.029418586489347656, "lambda": 113.06908697673376}</t>
         </is>
       </c>
-      <c r="Y77" t="inlineStr"/>
+      <c r="Y77" t="n">
+        <v>257.0125213383843</v>
+      </c>
       <c r="Z77" t="inlineStr">
         <is>
           <t>{"A": 11.502812995584057, "mu_m": 0.0227605053384196, "lambda": 48.17210750636222}</t>
@@ -17912,7 +18064,9 @@
           <t>{"A": 11.357642298248052, "mu_m": 0.030216616153689833, "lambda": 128.5611863123365}</t>
         </is>
       </c>
-      <c r="Y78" t="inlineStr"/>
+      <c r="Y78" t="n">
+        <v>266.8375267355315</v>
+      </c>
       <c r="Z78" t="inlineStr">
         <is>
           <t>{"A": 11.349532852695795, "mu_m": 0.02348476356723076, "lambda": 68.16245046506998}</t>
@@ -18135,7 +18289,9 @@
           <t>{"A": 11.47869556601469, "mu_m": 0.03402515093464879, "lambda": 159.9144669653347}</t>
         </is>
       </c>
-      <c r="Y79" t="inlineStr"/>
+      <c r="Y79" t="n">
+        <v>284.0219578714932</v>
+      </c>
       <c r="Z79" t="inlineStr">
         <is>
           <t>{"A": 11.471458471933746, "mu_m": 0.026405247052273227, "lambda": 105.48906472203105}</t>
@@ -18358,7 +18514,9 @@
           <t>{"A": 11.664127803220039, "mu_m": 0.032027059043237056, "lambda": 148.07282580731643}</t>
         </is>
       </c>
-      <c r="Y80" t="inlineStr"/>
+      <c r="Y80" t="n">
+        <v>282.0530583415607</v>
+      </c>
       <c r="Z80" t="inlineStr">
         <is>
           <t>{"A": 11.655912561013707, "mu_m": 0.024967409718666844, "lambda": 91.11777175341102}</t>
@@ -18581,7 +18739,9 @@
           <t>{"A": 11.837528659746063, "mu_m": 0.030649555411330177, "lambda": 140.08078005545008}</t>
         </is>
       </c>
-      <c r="Y81" t="inlineStr"/>
+      <c r="Y81" t="n">
+        <v>282.1638664087512</v>
+      </c>
       <c r="Z81" t="inlineStr">
         <is>
           <t>{"A": 11.827138896421156, "mu_m": 0.02415921500859633, "lambda": 83.92687808296633}</t>
@@ -18804,7 +18964,9 @@
           <t>{"A": 12.001280711508118, "mu_m": 0.034623945925586805, "lambda": 161.62332627736592}</t>
         </is>
       </c>
-      <c r="Y82" t="inlineStr"/>
+      <c r="Y82" t="n">
+        <v>289.1369392832293</v>
+      </c>
       <c r="Z82" t="inlineStr">
         <is>
           <t>{"A": 11.99254848039249, "mu_m": 0.027113428265985617, "lambda": 109.0329224951092}</t>
@@ -19027,7 +19189,9 @@
           <t>{"A": 11.749468182824506, "mu_m": 0.02986919726512329, "lambda": 129.7378098371352}</t>
         </is>
       </c>
-      <c r="Y83" t="inlineStr"/>
+      <c r="Y83" t="n">
+        <v>274.4483539737247</v>
+      </c>
       <c r="Z83" t="inlineStr">
         <is>
           <t>{"A": 11.739730199882505, "mu_m": 0.023389723265426945, "lambda": 69.78953549300114}</t>
@@ -19250,7 +19414,9 @@
           <t>{"A": 11.727820848908047, "mu_m": 0.03030659712555776, "lambda": 114.03832319020974}</t>
         </is>
       </c>
-      <c r="Y84" t="inlineStr"/>
+      <c r="Y84" t="n">
+        <v>256.3975647170884</v>
+      </c>
       <c r="Z84" t="inlineStr">
         <is>
           <t>{"A": 11.720002295747705, "mu_m": 0.023413279685609432, "lambda": 49.27956470290373}</t>
@@ -19473,7 +19639,9 @@
           <t>{"A": 11.703125070457922, "mu_m": 0.03466769692470743, "lambda": 162.58937673241059}</t>
         </is>
       </c>
-      <c r="Y85" t="inlineStr"/>
+      <c r="Y85" t="n">
+        <v>286.7781603204883</v>
+      </c>
       <c r="Z85" t="inlineStr">
         <is>
           <t>{"A": 11.695854386709174, "mu_m": 0.027118743944575766, "lambda": 111.23420586284179}</t>
@@ -19692,7 +19860,9 @@
           <t>{"A": 11.369644187070607, "mu_m": 0.03638489382379736, "lambda": 184.31596831573754}</t>
         </is>
       </c>
-      <c r="Y86" t="inlineStr"/>
+      <c r="Y86" t="n">
+        <v>299.2718719968973</v>
+      </c>
       <c r="Z86" t="inlineStr">
         <is>
           <t>{"A": 11.362464955244612, "mu_m": 0.028561401619822135, "lambda": 138.01890620273474}</t>
@@ -19915,7 +20085,9 @@
           <t>{"A": 11.549513225797783, "mu_m": 0.03154603667021181, "lambda": 147.60799256574995}</t>
         </is>
       </c>
-      <c r="Y87" t="inlineStr"/>
+      <c r="Y87" t="n">
+        <v>282.2945941102394</v>
+      </c>
       <c r="Z87" t="inlineStr">
         <is>
           <t>{"A": 11.54075469059237, "mu_m": 0.024816096724937176, "lambda": 93.80168426475225}</t>
@@ -20138,7 +20310,9 @@
           <t>{"A": 12.587243711106348, "mu_m": 0.028192162724972943, "lambda": 45.91606918224421}</t>
         </is>
       </c>
-      <c r="Y88" t="inlineStr"/>
+      <c r="Y88" t="n">
+        <v>210.1669720840187</v>
+      </c>
       <c r="Z88" t="inlineStr">
         <is>
           <t>{"A": 12.57873208992241, "mu_m": 0.02142765185423928, "lambda": -37.58731318741808}</t>
@@ -20361,7 +20535,9 @@
           <t>{"A": 12.369406612217503, "mu_m": 0.02745722722122624, "lambda": 41.96109444584093}</t>
         </is>
       </c>
-      <c r="Y89" t="inlineStr"/>
+      <c r="Y89" t="n">
+        <v>207.6897878591045</v>
+      </c>
       <c r="Z89" t="inlineStr">
         <is>
           <t>{"A": 12.361233564519123, "mu_m": 0.02083477137951406, "lambda": -43.12576600735149}</t>
@@ -20584,7 +20760,9 @@
           <t>{"A": 12.039338713916841, "mu_m": 0.026809500697159098, "lambda": 48.432105292003314}</t>
         </is>
       </c>
-      <c r="Y90" t="inlineStr"/>
+      <c r="Y90" t="n">
+        <v>213.6356742871829</v>
+      </c>
       <c r="Z90" t="inlineStr">
         <is>
           <t>{"A": 12.030614344232758, "mu_m": 0.020407871164992507, "lambda": -34.840402090610944}</t>
@@ -20807,7 +20985,9 @@
           <t>{"A": 12.241458631084402, "mu_m": 0.02675450886711418, "lambda": 39.00659817865353}</t>
         </is>
       </c>
-      <c r="Y91" t="inlineStr"/>
+      <c r="Y91" t="n">
+        <v>207.3289165846579</v>
+      </c>
       <c r="Z91" t="inlineStr">
         <is>
           <t>{"A": 12.2325662032811, "mu_m": 0.020352430230985874, "lambda": -46.24818144873123}</t>
@@ -21012,7 +21192,9 @@
           <t>{"A": 12.027223154358838, "mu_m": 0.024771231391164123, "lambda": 27.408519175919192}</t>
         </is>
       </c>
-      <c r="Y92" t="inlineStr"/>
+      <c r="Y92" t="n">
+        <v>206.0257248772071</v>
+      </c>
       <c r="Z92" t="inlineStr">
         <is>
           <t>{"A": 12.017568581586271, "mu_m": 0.01889614051986889, "lambda": -61.414237698577764}</t>
@@ -21235,7 +21417,9 @@
           <t>{"A": 12.093123865391805, "mu_m": 0.03542030924315539, "lambda": 137.63125889395292}</t>
         </is>
       </c>
-      <c r="Y93" t="inlineStr"/>
+      <c r="Y93" t="n">
+        <v>263.231846372648</v>
+      </c>
       <c r="Z93" t="inlineStr">
         <is>
           <t>{"A": 12.086221416843806, "mu_m": 0.02735320583940745, "lambda": 80.62590604344987}</t>
@@ -21458,7 +21642,9 @@
           <t>{"A": 11.74814206391112, "mu_m": 0.027217061298132478, "lambda": 39.221955690451715}</t>
         </is>
       </c>
-      <c r="Y94" t="inlineStr"/>
+      <c r="Y94" t="n">
+        <v>198.0157317683595</v>
+      </c>
       <c r="Z94" t="inlineStr">
         <is>
           <t>{"A": 11.742522284550047, "mu_m": 0.020500412730547184, "lambda": -45.791779037940394}</t>
@@ -21681,7 +21867,9 @@
           <t>{"A": 11.737443580988408, "mu_m": 0.030987749814133703, "lambda": 103.44305281265305}</t>
         </is>
       </c>
-      <c r="Y95" t="inlineStr"/>
+      <c r="Y95" t="n">
+        <v>242.7872843639836</v>
+      </c>
       <c r="Z95" t="inlineStr">
         <is>
           <t>{"A": 11.730867723787759, "mu_m": 0.023683965542700715, "lambda": 35.58442031214283}</t>
@@ -21904,7 +22092,9 @@
           <t>{"A": 11.746321987694245, "mu_m": 0.0279051756882337, "lambda": 53.43323429041574}</t>
         </is>
       </c>
-      <c r="Y96" t="inlineStr"/>
+      <c r="Y96" t="n">
+        <v>208.2873164481871</v>
+      </c>
       <c r="Z96" t="inlineStr">
         <is>
           <t>{"A": 11.740607937275502, "mu_m": 0.021067821354149932, "lambda": -28.196877059705272}</t>
@@ -22123,7 +22313,9 @@
           <t>{"A": 11.459679565997915, "mu_m": 0.028040111125258966, "lambda": 68.69599152788197}</t>
         </is>
       </c>
-      <c r="Y97" t="inlineStr"/>
+      <c r="Y97" t="n">
+        <v>219.0442014872023</v>
+      </c>
       <c r="Z97" t="inlineStr">
         <is>
           <t>{"A": 11.453230851981372, "mu_m": 0.02132878651159974, "lambda": -7.092832520803025}</t>
@@ -22342,7 +22534,9 @@
           <t>{"A": 11.231190548844847, "mu_m": 0.0329554455328474, "lambda": 128.74976316297887}</t>
         </is>
       </c>
-      <c r="Y98" t="inlineStr"/>
+      <c r="Y98" t="n">
+        <v>254.1227944175814</v>
+      </c>
       <c r="Z98" t="inlineStr">
         <is>
           <t>{"A": 11.225088157481729, "mu_m": 0.02528979133230866, "lambda": 69.21618371118264}</t>
@@ -22561,7 +22755,9 @@
           <t>{"A": 11.336272716320256, "mu_m": 0.03167654268954392, "lambda": 112.52596767525672}</t>
         </is>
       </c>
-      <c r="Y99" t="inlineStr"/>
+      <c r="Y99" t="n">
+        <v>244.1811711082867</v>
+      </c>
       <c r="Z99" t="inlineStr">
         <is>
           <t>{"A": 11.330026110761255, "mu_m": 0.024294517263388573, "lambda": 49.692997303815055}</t>
@@ -22784,7 +22980,9 @@
           <t>{"A": 12.152730349683425, "mu_m": 0.04264623131430335, "lambda": 169.48192843819635}</t>
         </is>
       </c>
-      <c r="Y100" t="inlineStr"/>
+      <c r="Y100" t="n">
+        <v>274.3150992006806</v>
+      </c>
       <c r="Z100" t="inlineStr">
         <is>
           <t>{"A": 12.147484950461472, "mu_m": 0.033097081410795606, "lambda": 123.75115644611478}</t>
@@ -23003,7 +23201,9 @@
           <t>{"A": 11.389742599398957, "mu_m": 0.036705870317370576, "lambda": 125.24582181813582}</t>
         </is>
       </c>
-      <c r="Y101" t="inlineStr"/>
+      <c r="Y101" t="n">
+        <v>239.3979208236884</v>
+      </c>
       <c r="Z101" t="inlineStr">
         <is>
           <t>{"A": 11.385921443053052, "mu_m": 0.027802412189672384, "lambda": 66.46118319386595}</t>
@@ -23222,7 +23422,9 @@
           <t>{"A": 11.38912335646127, "mu_m": 0.039426632523540686, "lambda": 156.20241963083075}</t>
         </is>
       </c>
-      <c r="Y102" t="inlineStr"/>
+      <c r="Y102" t="n">
+        <v>262.4713061076545</v>
+      </c>
       <c r="Z102" t="inlineStr">
         <is>
           <t>{"A": 11.384411911697171, "mu_m": 0.03031946362271711, "lambda": 106.62388594298064}</t>
@@ -23441,7 +23643,9 @@
           <t>{"A": 11.487904182051631, "mu_m": 0.035755777355890465, "lambda": 108.2304989353327}</t>
         </is>
       </c>
-      <c r="Y103" t="inlineStr"/>
+      <c r="Y103" t="n">
+        <v>226.4257692733164</v>
+      </c>
       <c r="Z103" t="inlineStr">
         <is>
           <t>{"A": 11.484648470413047, "mu_m": 0.026766522291905095, "lambda": 42.76598600005699}</t>
@@ -23664,7 +23868,9 @@
           <t>{"A": 12.023960204001492, "mu_m": 0.04017880747258386, "lambda": 137.79089423408064}</t>
         </is>
       </c>
-      <c r="Y104" t="inlineStr"/>
+      <c r="Y104" t="n">
+        <v>247.882956163346</v>
+      </c>
       <c r="Z104" t="inlineStr">
         <is>
           <t>{"A": 12.01966674313645, "mu_m": 0.030649739240937876, "lambda": 83.63052251437644}</t>
@@ -23887,7 +24093,9 @@
           <t>{"A": 11.696151036313461, "mu_m": 0.040340356553933775, "lambda": 145.8285779134721}</t>
         </is>
       </c>
-      <c r="Y105" t="inlineStr"/>
+      <c r="Y105" t="n">
+        <v>252.4903398476561</v>
+      </c>
       <c r="Z105" t="inlineStr">
         <is>
           <t>{"A": 11.692290430517609, "mu_m": 0.030686925479069364, "lambda": 92.51100583069393}</t>
@@ -24210,7 +24418,9 @@
           <t>{"A": 11.975555950223802, "mu_m": 0.033401047628991404, "lambda": 118.15202035161082}</t>
         </is>
       </c>
-      <c r="Y106" t="inlineStr"/>
+      <c r="Y106" t="n">
+        <v>250.0509020759595</v>
+      </c>
       <c r="Z106" t="inlineStr">
         <is>
           <t>{"A": 11.973799695755492, "mu_m": 0.024775082358680887, "lambda": 40.56737854255852}</t>
@@ -24533,7 +24743,9 @@
           <t>{"A": 12.044899446704422, "mu_m": 0.03531165917212819, "lambda": 132.18193309226228}</t>
         </is>
       </c>
-      <c r="Y107" t="inlineStr"/>
+      <c r="Y107" t="n">
+        <v>257.6665741797964</v>
+      </c>
       <c r="Z107" t="inlineStr">
         <is>
           <t>{"A": 12.043191017897863, "mu_m": 0.026235250482132887, "lambda": 59.11542351596839}</t>
@@ -24856,7 +25068,9 @@
           <t>{"A": 12.139836564910672, "mu_m": 0.034181898450791406, "lambda": 139.97828363982524}</t>
         </is>
       </c>
-      <c r="Y108" t="inlineStr"/>
+      <c r="Y108" t="n">
+        <v>270.6321236493634</v>
+      </c>
       <c r="Z108" t="inlineStr">
         <is>
           <t>{"A": 12.137640772385272, "mu_m": 0.02566929726581736, "lambda": 68.78788438168553}</t>
@@ -25179,7 +25393,9 @@
           <t>{"A": 11.900944744796716, "mu_m": 0.03566159745624477, "lambda": 155.67477494714763}</t>
         </is>
       </c>
-      <c r="Y109" t="inlineStr"/>
+      <c r="Y109" t="n">
+        <v>278.4430527142831</v>
+      </c>
       <c r="Z109" t="inlineStr">
         <is>
           <t>{"A": 11.898865117642584, "mu_m": 0.026826036664573016, "lambda": 89.48017747349657}</t>
@@ -25502,7 +25718,9 @@
           <t>{"A": 11.698252208935456, "mu_m": 0.03333155786511885, "lambda": 189.62709158161456}</t>
         </is>
       </c>
-      <c r="Y110" t="inlineStr"/>
+      <c r="Y110" t="n">
+        <v>318.7403632360842</v>
+      </c>
       <c r="Z110" t="inlineStr">
         <is>
           <t>{"A": 11.694666121194132, "mu_m": 0.025890308522803784, "lambda": 133.31440551477974}</t>
@@ -25825,7 +26043,9 @@
           <t>{"A": 12.360390754681974, "mu_m": 0.031067087702033824, "lambda": 109.41522124398134}</t>
         </is>
       </c>
-      <c r="Y111" t="inlineStr"/>
+      <c r="Y111" t="n">
+        <v>255.7802003854084</v>
+      </c>
       <c r="Z111" t="inlineStr">
         <is>
           <t>{"A": 12.357851706007326, "mu_m": 0.023288321156093354, "lambda": 28.67233075368828}</t>
@@ -26148,7 +26368,9 @@
           <t>{"A": 12.495406648382444, "mu_m": 0.03259381846059773, "lambda": 135.22899856775484}</t>
         </is>
       </c>
-      <c r="Y112" t="inlineStr"/>
+      <c r="Y112" t="n">
+        <v>276.2619745160586</v>
+      </c>
       <c r="Z112" t="inlineStr">
         <is>
           <t>{"A": 12.492456538072107, "mu_m": 0.024692281687861996, "lambda": 62.44434434077438}</t>
@@ -26471,7 +26693,9 @@
           <t>{"A": 12.44016203560402, "mu_m": 0.0329309976802279, "lambda": 121.13996817869341}</t>
         </is>
       </c>
-      <c r="Y113" t="inlineStr"/>
+      <c r="Y113" t="n">
+        <v>260.1117631476616</v>
+      </c>
       <c r="Z113" t="inlineStr">
         <is>
           <t>{"A": 12.437788341621628, "mu_m": 0.024671228132262045, "lambda": 44.209522014145605}</t>
@@ -26788,7 +27012,9 @@
           <t>{"A": 11.29054679663199, "mu_m": 0.019224127356545818, "lambda": 216.97532749184572}</t>
         </is>
       </c>
-      <c r="Y114" t="inlineStr"/>
+      <c r="Y114" t="n">
+        <v>433.0350720529276</v>
+      </c>
       <c r="Z114" t="inlineStr">
         <is>
           <t>{"A": 11.273526863736357, "mu_m": 0.016340500235203174, "lambda": 173.74014197581118}</t>
@@ -27111,7 +27337,9 @@
           <t>{"A": 11.723194539676223, "mu_m": 0.019533614435044568, "lambda": 93.2759388703943}</t>
         </is>
       </c>
-      <c r="Y115" t="inlineStr"/>
+      <c r="Y115" t="n">
+        <v>314.0605903920754</v>
+      </c>
       <c r="Z115" t="inlineStr">
         <is>
           <t>{"A": 11.715506002516086, "mu_m": 0.015391378759768847, "lambda": 6.496659663015217}</t>
@@ -27434,7 +27662,9 @@
           <t>{"A": 11.900729308581415, "mu_m": 0.020762508941240744, "lambda": 97.61886044762312}</t>
         </is>
       </c>
-      <c r="Y116" t="inlineStr"/>
+      <c r="Y116" t="n">
+        <v>308.4813173868908</v>
+      </c>
       <c r="Z116" t="inlineStr">
         <is>
           <t>{"A": 11.893309744380618, "mu_m": 0.016307905924995078, "lambda": 12.522455987120331}</t>
@@ -27757,7 +27987,9 @@
           <t>{"A": 11.93640484504342, "mu_m": 0.02182199263935224, "lambda": 119.18784642873545}</t>
         </is>
       </c>
-      <c r="Y117" t="inlineStr"/>
+      <c r="Y117" t="n">
+        <v>320.4141054859384</v>
+      </c>
       <c r="Z117" t="inlineStr">
         <is>
           <t>{"A": 11.928964902630252, "mu_m": 0.017217262050597, "lambda": 40.666462820262076}</t>
@@ -28080,7 +28312,9 @@
           <t>{"A": 12.716843649786012, "mu_m": 0.017270557153475908, "lambda": 54.71143597688829}</t>
         </is>
       </c>
-      <c r="Y118" t="inlineStr"/>
+      <c r="Y118" t="n">
+        <v>325.5924095189797</v>
+      </c>
       <c r="Z118" t="inlineStr">
         <is>
           <t>{"A": 12.701373470972149, "mu_m": 0.013821733251908433, "lambda": -41.655898178650126}</t>
@@ -28403,7 +28637,9 @@
           <t>{"A": 12.37864050425792, "mu_m": 0.019546856152963973, "lambda": 141.05392484977133}</t>
         </is>
       </c>
-      <c r="Y119" t="inlineStr"/>
+      <c r="Y119" t="n">
+        <v>374.0247573730396</v>
+      </c>
       <c r="Z119" t="inlineStr">
         <is>
           <t>{"A": 12.363623343877316, "mu_m": 0.015874188750602085, "lambda": 67.76274793425469}</t>
@@ -28726,7 +28962,9 @@
           <t>{"A": 12.370770567979102, "mu_m": 0.020041339573858296, "lambda": 148.13072986935921}</t>
         </is>
       </c>
-      <c r="Y120" t="inlineStr"/>
+      <c r="Y120" t="n">
+        <v>375.2089721513517</v>
+      </c>
       <c r="Z120" t="inlineStr">
         <is>
           <t>{"A": 12.358539398333978, "mu_m": 0.016046736346202774, "lambda": 68.96416870339431}</t>
@@ -29049,7 +29287,9 @@
           <t>{"A": 12.525371486654645, "mu_m": 0.022334085903871183, "lambda": 194.9478237353793}</t>
         </is>
       </c>
-      <c r="Y121" t="inlineStr"/>
+      <c r="Y121" t="n">
+        <v>401.2614683952913</v>
+      </c>
       <c r="Z121" t="inlineStr">
         <is>
           <t>{"A": 12.513908882954862, "mu_m": 0.01805001010813354, "lambda": 129.57276956275766}</t>
@@ -29372,7 +29612,9 @@
           <t>{"A": 12.920074401057938, "mu_m": 0.018286081684930056, "lambda": 59.29748399503753}</t>
         </is>
       </c>
-      <c r="Y122" t="inlineStr"/>
+      <c r="Y122" t="n">
+        <v>319.2235760058658</v>
+      </c>
       <c r="Z122" t="inlineStr">
         <is>
           <t>{"A": 12.906938292033171, "mu_m": 0.014566975776648632, "lambda": -35.8271932912135}</t>
@@ -29695,7 +29937,9 @@
           <t>{"A": 12.929876895165233, "mu_m": 0.018883516371142828, "lambda": 65.91695934374337}</t>
         </is>
       </c>
-      <c r="Y123" t="inlineStr"/>
+      <c r="Y123" t="n">
+        <v>317.8105046517489</v>
+      </c>
       <c r="Z123" t="inlineStr">
         <is>
           <t>{"A": 12.917615424589279, "mu_m": 0.015035515961791932, "lambda": -26.47902143094266}</t>
@@ -30023,7 +30267,9 @@
           <t>{"A": 11.533695779671358, "mu_m": 0.03659893758440516, "lambda": 91.75540638182518}</t>
         </is>
       </c>
-      <c r="Y124" t="inlineStr"/>
+      <c r="Y124" t="n">
+        <v>207.6879945418398</v>
+      </c>
       <c r="Z124" t="inlineStr">
         <is>
           <t>{"A": 11.531592069542768, "mu_m": 0.027621903357167927, "lambda": 30.464729450030166}</t>
@@ -30344,7 +30590,9 @@
           <t>{"A": 11.435631995198756, "mu_m": 0.03209979292559707, "lambda": 39.778305654581494}</t>
         </is>
       </c>
-      <c r="Y125" t="inlineStr"/>
+      <c r="Y125" t="n">
+        <v>170.8362821838096</v>
+      </c>
       <c r="Z125" t="inlineStr">
         <is>
           <t>{"A": 11.433861659727537, "mu_m": 0.023856767242317174, "lambda": -36.477997731122926}</t>
@@ -30672,7 +30920,9 @@
           <t>{"A": 11.611586443855844, "mu_m": 0.0359095355319132, "lambda": 80.87300300354845}</t>
         </is>
       </c>
-      <c r="Y126" t="inlineStr"/>
+      <c r="Y126" t="n">
+        <v>199.8292598530225</v>
+      </c>
       <c r="Z126" t="inlineStr">
         <is>
           <t>{"A": 11.609566871651085, "mu_m": 0.027044057696533057, "lambda": 17.147374176430876}</t>
@@ -31000,7 +31250,9 @@
           <t>{"A": 11.712074204438295, "mu_m": 0.033876053733115, "lambda": 58.790494878018514}</t>
         </is>
       </c>
-      <c r="Y127" t="inlineStr"/>
+      <c r="Y127" t="n">
+        <v>185.978606788332</v>
+      </c>
       <c r="Z127" t="inlineStr">
         <is>
           <t>{"A": 11.710199573822011, "mu_m": 0.02534406259718324, "lambda": -12.122799859048651}</t>
@@ -31328,7 +31580,9 @@
           <t>{"A": 11.596554971926738, "mu_m": 0.032677719448933294, "lambda": 52.76444387890838}</t>
         </is>
       </c>
-      <c r="Y128" t="inlineStr"/>
+      <c r="Y128" t="n">
+        <v>183.3162153773193</v>
+      </c>
       <c r="Z128" t="inlineStr">
         <is>
           <t>{"A": 11.594700909216561, "mu_m": 0.024421357280780622, "lambda": -20.462289224788922}</t>
@@ -31649,7 +31903,9 @@
           <t>{"A": 11.475661008940763, "mu_m": 0.03420832199592667, "lambda": 100.74983874825341}</t>
         </is>
       </c>
-      <c r="Y129" t="inlineStr"/>
+      <c r="Y129" t="n">
+        <v>224.1601527515164</v>
+      </c>
       <c r="Z129" t="inlineStr">
         <is>
           <t>{"A": 11.472701270970573, "mu_m": 0.02633146317426359, "lambda": 43.34036347070504}</t>
@@ -31970,7 +32226,9 @@
           <t>{"A": 11.49280472685575, "mu_m": 0.033272965332543245, "lambda": 85.72630154382144}</t>
         </is>
       </c>
-      <c r="Y130" t="inlineStr"/>
+      <c r="Y130" t="n">
+        <v>212.795426226645</v>
+      </c>
       <c r="Z130" t="inlineStr">
         <is>
           <t>{"A": 11.490166775013114, "mu_m": 0.025397975737498083, "lambda": 23.323034387225995}</t>
@@ -32298,7 +32556,9 @@
           <t>{"A": 12.225312927960223, "mu_m": 0.04174534246438694, "lambda": 96.03841496787469}</t>
         </is>
       </c>
-      <c r="Y131" t="inlineStr"/>
+      <c r="Y131" t="n">
+        <v>203.7735782838972</v>
+      </c>
       <c r="Z131" t="inlineStr">
         <is>
           <t>{"A": 12.223547831336697, "mu_m": 0.0313029807672523, "lambda": 36.76944738577292}</t>
@@ -32626,7 +32886,9 @@
           <t>{"A": 12.026825806952292, "mu_m": 0.041505113825769796, "lambda": 96.4273392620057}</t>
         </is>
       </c>
-      <c r="Y132" t="inlineStr"/>
+      <c r="Y132" t="n">
+        <v>203.0267808513176</v>
+      </c>
       <c r="Z132" t="inlineStr">
         <is>
           <t>{"A": 12.025191378924108, "mu_m": 0.031073577193337348, "lambda": 37.242677626783866}</t>
@@ -32954,7 +33216,9 @@
           <t>{"A": 11.747064275801725, "mu_m": 0.038194101419378554, "lambda": 103.8675454725409}</t>
         </is>
       </c>
-      <c r="Y133" t="inlineStr"/>
+      <c r="Y133" t="n">
+        <v>217.0133790067827</v>
+      </c>
       <c r="Z133" t="inlineStr">
         <is>
           <t>{"A": 11.744725202860986, "mu_m": 0.029080512640273004, "lambda": 47.31889443657522}</t>
@@ -33282,7 +33546,9 @@
           <t>{"A": 12.024843096100167, "mu_m": 0.026082595110851578, "lambda": 173.87546284482872}</t>
         </is>
       </c>
-      <c r="Y134" t="inlineStr"/>
+      <c r="Y134" t="n">
+        <v>343.4786997760781</v>
+      </c>
       <c r="Z134" t="inlineStr">
         <is>
           <t>{"A": 12.013724821912527, "mu_m": 0.021672434902190493, "lambda": 132.20997027631384}</t>
@@ -33603,7 +33869,9 @@
           <t>{"A": 11.193135966599055, "mu_m": 0.020689154059026153, "lambda": 153.12403296786167}</t>
         </is>
       </c>
-      <c r="Y135" t="inlineStr"/>
+      <c r="Y135" t="n">
+        <v>352.1522094027495</v>
+      </c>
       <c r="Z135" t="inlineStr">
         <is>
           <t>{"A": 11.182812547430018, "mu_m": 0.01693296942339802, "lambda": 95.89668104265193}</t>
@@ -33924,7 +34192,9 @@
           <t>{"A": 10.815781745319088, "mu_m": 0.01763278564751686, "lambda": 75.31739499850717}</t>
         </is>
       </c>
-      <c r="Y136" t="inlineStr"/>
+      <c r="Y136" t="n">
+        <v>300.9711189102819</v>
+      </c>
       <c r="Z136" t="inlineStr">
         <is>
           <t>{"A": 10.807501774362825, "mu_m": 0.014094325542221283, "lambda": -3.3526262984782598}</t>
@@ -34245,7 +34515,9 @@
           <t>{"A": 10.865480773869615, "mu_m": 0.01764267316675155, "lambda": 90.70132898302097}</t>
         </is>
       </c>
-      <c r="Y137" t="inlineStr"/>
+      <c r="Y137" t="n">
+        <v>317.26489774442</v>
+      </c>
       <c r="Z137" t="inlineStr">
         <is>
           <t>{"A": 10.856917536804833, "mu_m": 0.014220887049596887, "lambda": 18.4740613795779}</t>
@@ -34566,7 +34838,9 @@
           <t>{"A": 10.876423991913422, "mu_m": 0.016065946845838935, "lambda": 37.74866040055607}</t>
         </is>
       </c>
-      <c r="Y138" t="inlineStr"/>
+      <c r="Y138" t="n">
+        <v>286.7979581781775</v>
+      </c>
       <c r="Z138" t="inlineStr">
         <is>
           <t>{"A": 10.866953511845981, "mu_m": 0.012906413049768965, "lambda": -45.301046396154426}</t>
@@ -34887,7 +35161,9 @@
           <t>{"A": 11.115432103261025, "mu_m": 0.022684220655202654, "lambda": 248.01458983285198}</t>
         </is>
       </c>
-      <c r="Y139" t="inlineStr"/>
+      <c r="Y139" t="n">
+        <v>428.2781753745896</v>
+      </c>
       <c r="Z139" t="inlineStr">
         <is>
           <t>{"A": 11.105820487571771, "mu_m": 0.018436268004666335, "lambda": 191.67983231885768}</t>
@@ -35208,7 +35484,9 @@
           <t>{"A": 11.253608072497492, "mu_m": 0.022550616675583366, "lambda": 182.28732054768375}</t>
         </is>
       </c>
-      <c r="Y140" t="inlineStr"/>
+      <c r="Y140" t="n">
+        <v>365.873033897836</v>
+      </c>
       <c r="Z140" t="inlineStr">
         <is>
           <t>{"A": 11.240782758572122, "mu_m": 0.01901527452430991, "lambda": 143.74363788857693}</t>
@@ -35536,7 +35814,9 @@
           <t>{"A": 11.62216148364922, "mu_m": 0.02406720077021123, "lambda": 152.39205352115732}</t>
         </is>
       </c>
-      <c r="Y141" t="inlineStr"/>
+      <c r="Y141" t="n">
+        <v>330.0427206108311</v>
+      </c>
       <c r="Z141" t="inlineStr">
         <is>
           <t>{"A": 11.61217120647053, "mu_m": 0.019891613551040348, "lambda": 105.98377102907972}</t>
@@ -35857,7 +36137,9 @@
           <t>{"A": 11.381361060412493, "mu_m": 0.024399268101104547, "lambda": 181.34857132101243}</t>
         </is>
       </c>
-      <c r="Y142" t="inlineStr"/>
+      <c r="Y142" t="n">
+        <v>352.9507984585313</v>
+      </c>
       <c r="Z142" t="inlineStr">
         <is>
           <t>{"A": 11.371800975884597, "mu_m": 0.02016377831610914, "lambda": 136.38007925093936}</t>
@@ -36178,7 +36460,9 @@
           <t>{"A": 11.32406422254952, "mu_m": 0.028158603753318957, "lambda": 258.7663493247827}</t>
         </is>
       </c>
-      <c r="Y143" t="inlineStr"/>
+      <c r="Y143" t="n">
+        <v>406.7101342679556</v>
+      </c>
       <c r="Z143" t="inlineStr">
         <is>
           <t>{"A": 11.314024215635527, "mu_m": 0.02348151719400667, "lambda": 222.78493969045277}</t>
@@ -36499,7 +36783,9 @@
           <t>{"A": 11.256635508384193, "mu_m": 0.022402706810979216, "lambda": 47.72407762613267}</t>
         </is>
       </c>
-      <c r="Y144" t="inlineStr"/>
+      <c r="Y144" t="n">
+        <v>232.5715969564982</v>
+      </c>
       <c r="Z144" t="inlineStr">
         <is>
           <t>{"A": 11.250592928301925, "mu_m": 0.017649894130582308, "lambda": -25.288794925245565}</t>
@@ -36820,7 +37106,9 @@
           <t>{"A": 11.410989167323399, "mu_m": 0.023490739146387996, "lambda": 50.28346345745062}</t>
         </is>
       </c>
-      <c r="Y145" t="inlineStr"/>
+      <c r="Y145" t="n">
+        <v>228.9865809680715</v>
+      </c>
       <c r="Z145" t="inlineStr">
         <is>
           <t>{"A": 11.405347359122375, "mu_m": 0.018454615722155936, "lambda": -21.76688552237678}</t>
@@ -37141,7 +37429,9 @@
           <t>{"A": 11.493888861142171, "mu_m": 0.02444650644706735, "lambda": 85.43828996455314}</t>
         </is>
       </c>
-      <c r="Y146" t="inlineStr"/>
+      <c r="Y146" t="n">
+        <v>258.4022846473553</v>
+      </c>
       <c r="Z146" t="inlineStr">
         <is>
           <t>{"A": 11.4878013706267, "mu_m": 0.019350627670684153, "lambda": 19.92667916843899}</t>

</xml_diff>